<commit_message>
report diagrams and results
</commit_message>
<xml_diff>
--- a/Reports/Results.xlsx
+++ b/Reports/Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="43">
   <si>
     <t>Euclidean</t>
   </si>
@@ -804,11 +804,11 @@
         </c:dLbls>
         <c:gapWidth val="180"/>
         <c:overlap val="-27"/>
-        <c:axId val="133644640"/>
-        <c:axId val="133996736"/>
+        <c:axId val="140332376"/>
+        <c:axId val="140333160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133644640"/>
+        <c:axId val="140332376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -914,7 +914,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133996736"/>
+        <c:crossAx val="140333160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -924,7 +924,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133996736"/>
+        <c:axId val="140333160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,7 +1038,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133644640"/>
+        <c:crossAx val="140332376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1362,8 +1362,8 @@
         </c:dLbls>
         <c:gapWidth val="180"/>
         <c:overlap val="-27"/>
-        <c:axId val="134173944"/>
-        <c:axId val="134175904"/>
+        <c:axId val="141070304"/>
+        <c:axId val="141071088"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2001,7 +2001,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134173944"/>
+        <c:axId val="141070304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2107,7 +2107,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134175904"/>
+        <c:crossAx val="141071088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2117,7 +2117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134175904"/>
+        <c:axId val="141071088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,7 +2231,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134173944"/>
+        <c:crossAx val="141070304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2873,11 +2873,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="133997128"/>
-        <c:axId val="133995952"/>
+        <c:axId val="140333552"/>
+        <c:axId val="140334728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133997128"/>
+        <c:axId val="140333552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2980,7 +2980,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133995952"/>
+        <c:crossAx val="140334728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2988,7 +2988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133995952"/>
+        <c:axId val="140334728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3102,7 +3102,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133997128"/>
+        <c:crossAx val="140333552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3281,11 +3281,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="133995560"/>
-        <c:axId val="133997912"/>
+        <c:axId val="140331592"/>
+        <c:axId val="140331984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133995560"/>
+        <c:axId val="140331592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3401,7 +3401,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133997912"/>
+        <c:crossAx val="140331984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3409,7 +3409,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133997912"/>
+        <c:axId val="140331984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3533,7 +3533,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133995560"/>
+        <c:crossAx val="140331592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3671,11 +3671,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="133998696"/>
-        <c:axId val="133999088"/>
+        <c:axId val="140334336"/>
+        <c:axId val="140934960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133998696"/>
+        <c:axId val="140334336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3791,7 +3791,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133999088"/>
+        <c:crossAx val="140934960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3799,7 +3799,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133999088"/>
+        <c:axId val="140934960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3925,7 +3925,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133998696"/>
+        <c:crossAx val="140334336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4092,11 +4092,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="134174728"/>
-        <c:axId val="134178648"/>
+        <c:axId val="140933000"/>
+        <c:axId val="140935352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134174728"/>
+        <c:axId val="140933000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4212,7 +4212,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134178648"/>
+        <c:crossAx val="140935352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4220,7 +4220,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134178648"/>
+        <c:axId val="140935352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
@@ -4346,7 +4346,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134174728"/>
+        <c:crossAx val="140933000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4513,11 +4513,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="134172376"/>
-        <c:axId val="134175120"/>
+        <c:axId val="140937312"/>
+        <c:axId val="140934568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134172376"/>
+        <c:axId val="140937312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4633,7 +4633,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134175120"/>
+        <c:crossAx val="140934568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4641,7 +4641,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134175120"/>
+        <c:axId val="140934568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.9"/>
@@ -4766,7 +4766,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134172376"/>
+        <c:crossAx val="140937312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4995,11 +4995,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="134177864"/>
-        <c:axId val="134176688"/>
+        <c:axId val="140931040"/>
+        <c:axId val="140933392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134177864"/>
+        <c:axId val="140931040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5115,7 +5115,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134176688"/>
+        <c:crossAx val="140933392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5123,7 +5123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134176688"/>
+        <c:axId val="140933392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5247,7 +5247,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134177864"/>
+        <c:crossAx val="140931040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5507,11 +5507,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="134172768"/>
-        <c:axId val="134179432"/>
+        <c:axId val="140937704"/>
+        <c:axId val="140932216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134172768"/>
+        <c:axId val="140937704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5627,7 +5627,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134179432"/>
+        <c:crossAx val="140932216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5635,7 +5635,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134179432"/>
+        <c:axId val="140932216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5759,7 +5759,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134172768"/>
+        <c:crossAx val="140937704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6081,8 +6081,8 @@
         </c:dLbls>
         <c:gapWidth val="180"/>
         <c:overlap val="-27"/>
-        <c:axId val="134179824"/>
-        <c:axId val="134173160"/>
+        <c:axId val="141073048"/>
+        <c:axId val="141074224"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -6720,7 +6720,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134179824"/>
+        <c:axId val="141073048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6826,7 +6826,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134173160"/>
+        <c:crossAx val="141074224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6836,7 +6836,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134173160"/>
+        <c:axId val="141074224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6950,7 +6950,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134179824"/>
+        <c:crossAx val="141073048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14469,20 +14469,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:Y26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17:Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -14493,7 +14493,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -14503,8 +14503,26 @@
       <c r="D4" s="3">
         <v>0.81220000000000003</v>
       </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0.86519999999999997</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -14514,8 +14532,26 @@
       <c r="D5" s="3">
         <v>0.83209999999999995</v>
       </c>
+      <c r="T5" s="1">
+        <v>3</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.83479999999999999</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0.89380000000000004</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -14525,8 +14561,26 @@
       <c r="D6" s="3">
         <v>0.83379999999999999</v>
       </c>
+      <c r="T6" s="1">
+        <v>4</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0.83750000000000002</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0.89759999999999995</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -14536,8 +14590,26 @@
       <c r="D7" s="3">
         <v>0.83679999999999999</v>
       </c>
+      <c r="T7" s="1">
+        <v>6</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="3">
+        <v>0.83779999999999999</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0.90290000000000004</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>8</v>
       </c>
@@ -14547,8 +14619,26 @@
       <c r="D8" s="3">
         <v>0.83919999999999995</v>
       </c>
+      <c r="T8" s="1">
+        <v>8</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0.91239999999999999</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>10</v>
       </c>
@@ -14558,8 +14648,26 @@
       <c r="D9" s="3">
         <v>0.83799999999999997</v>
       </c>
+      <c r="T9" s="1">
+        <v>10</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0.8397</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0.91449999999999998</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>12</v>
       </c>
@@ -14569,8 +14677,26 @@
       <c r="D10" s="3">
         <v>0.8387</v>
       </c>
+      <c r="T10" s="1">
+        <v>12</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0.8407</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0.91510000000000002</v>
+      </c>
+      <c r="Y10" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>14</v>
       </c>
@@ -14580,8 +14706,26 @@
       <c r="D11" s="3">
         <v>0.83650000000000002</v>
       </c>
+      <c r="T11" s="1">
+        <v>14</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0.83750000000000002</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0.91239999999999999</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>17</v>
       </c>
@@ -14591,8 +14735,26 @@
       <c r="D12" s="3">
         <v>0.83279999999999998</v>
       </c>
+      <c r="T12" s="1">
+        <v>17</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V12" s="3">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X12" s="3">
+        <v>0.91080000000000005</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>20</v>
       </c>
@@ -14602,13 +14764,31 @@
       <c r="D13" s="3">
         <v>0.83430000000000004</v>
       </c>
+      <c r="T13" s="1">
+        <v>20</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V13" s="3">
+        <v>0.83379999999999999</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X13" s="3">
+        <v>0.91349999999999998</v>
+      </c>
+      <c r="Y13" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
@@ -14619,7 +14799,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>1</v>
       </c>
@@ -14629,8 +14809,26 @@
       <c r="D17" s="3">
         <v>0.86939999999999995</v>
       </c>
+      <c r="T17" s="1">
+        <v>1</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V17" s="3">
+        <v>0.81220000000000003</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X17" s="3">
+        <v>0.86939999999999995</v>
+      </c>
+      <c r="Y17" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>3</v>
       </c>
@@ -14640,8 +14838,26 @@
       <c r="D18" s="3">
         <v>0.9002</v>
       </c>
+      <c r="T18" s="1">
+        <v>3</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0.83209999999999995</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0.9002</v>
+      </c>
+      <c r="Y18" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>4</v>
       </c>
@@ -14651,8 +14867,26 @@
       <c r="D19" s="3">
         <v>0.90290000000000004</v>
       </c>
+      <c r="T19" s="1">
+        <v>4</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V19" s="3">
+        <v>0.83379999999999999</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X19" s="3">
+        <v>0.90290000000000004</v>
+      </c>
+      <c r="Y19" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>6</v>
       </c>
@@ -14662,8 +14896,26 @@
       <c r="D20" s="3">
         <v>0.90500000000000003</v>
       </c>
+      <c r="T20" s="1">
+        <v>6</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V20" s="3">
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X20" s="3">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="Y20" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>8</v>
       </c>
@@ -14673,8 +14925,26 @@
       <c r="D21" s="3">
         <v>0.91080000000000005</v>
       </c>
+      <c r="T21" s="1">
+        <v>8</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V21" s="3">
+        <v>0.83919999999999995</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X21" s="3">
+        <v>0.91080000000000005</v>
+      </c>
+      <c r="Y21" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>10</v>
       </c>
@@ -14684,8 +14954,26 @@
       <c r="D22" s="3">
         <v>0.91190000000000004</v>
       </c>
+      <c r="T22" s="1">
+        <v>10</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V22" s="3">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0.91190000000000004</v>
+      </c>
+      <c r="Y22" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>12</v>
       </c>
@@ -14695,8 +14983,26 @@
       <c r="D23" s="3">
         <v>0.91080000000000005</v>
       </c>
+      <c r="T23" s="1">
+        <v>12</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V23" s="3">
+        <v>0.8387</v>
+      </c>
+      <c r="W23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X23" s="3">
+        <v>0.91080000000000005</v>
+      </c>
+      <c r="Y23" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>14</v>
       </c>
@@ -14706,8 +15012,26 @@
       <c r="D24" s="3">
         <v>0.91300000000000003</v>
       </c>
+      <c r="T24" s="1">
+        <v>14</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V24" s="3">
+        <v>0.83650000000000002</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X24" s="3">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="Y24" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>17</v>
       </c>
@@ -14717,8 +15041,26 @@
       <c r="D25" s="3">
         <v>0.9103</v>
       </c>
+      <c r="T25" s="1">
+        <v>17</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V25" s="3">
+        <v>0.83279999999999998</v>
+      </c>
+      <c r="W25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X25" s="3">
+        <v>0.9103</v>
+      </c>
+      <c r="Y25" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>20</v>
       </c>
@@ -14728,9 +15070,33 @@
       <c r="D26" s="3">
         <v>0.91510000000000002</v>
       </c>
+      <c r="T26" s="1">
+        <v>20</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V26" s="3">
+        <v>0.83430000000000004</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X26" s="3">
+        <v>0.91510000000000002</v>
+      </c>
+      <c r="Y26" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Y4" r:id="rId1"/>
+    <hyperlink ref="Y5:Y13" r:id="rId2" display="\\"/>
+    <hyperlink ref="Y17" r:id="rId3"/>
+    <hyperlink ref="Y18:Y26" r:id="rId4" display="\\"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>